<commit_message>
Cambios en el metodo de encriptacion y agregadas las funcionalidades restantes
</commit_message>
<xml_diff>
--- a/Password.xlsx
+++ b/Password.xlsx
@@ -1,65 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Vscode\Python\Excel-passwords\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>Email/Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Counter:</t>
-  </si>
-  <si>
-    <t>El valor de counter indica la posicion libre en la que se pondra el siguiente dominio, email etc</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -78,27 +54,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -386,59 +421,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="2" customWidth="1"/>
+    <col width="18.42578125" customWidth="1" style="4" min="2" max="2"/>
+    <col width="16.42578125" customWidth="1" style="4" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Domain</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email/Username</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Counter:</t>
+        </is>
+      </c>
+      <c r="F1" t="n">
         <v>3</v>
       </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B4"/>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5"/>
-      <c r="C5"/>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>El valor de counter indica la posicion libre en la que se pondra el siguiente dominio, email etc</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se mejoro el ui de la aplicacion, y se hicieron mejoras en el codigo
</commit_message>
<xml_diff>
--- a/Password.xlsx
+++ b/Password.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -460,11 +460,96 @@
         </is>
       </c>
       <c r="F1" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H1" s="3" t="inlineStr">
         <is>
           <t>El valor de counter indica la posicion libre en la que se pondra el siguiente dominio, email etc</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>37V9#A1&gt;P0%j4-i3/i4#X3[c4)g6%F2|b9)g9+i2`X2$T7)E0(s5-U6(K3]Y6;,87V9#90A1&gt;139P0%92j4-73i3/158i4#93X3[163c4)159g6%86F2|101b9)123g9+91i2`79X2$154T7)88E0(74s5-108U6(89K3]162Y6;,124f7$122y8~134z1@130V6*133u3%136G4},</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>51m0&gt;z2:n6]j2{L0?p4}l4@j8/B7}u2?o1;N7[S1:F3$t0&amp;Q9{u9;X7=F4}l0*(108m0&gt;101z2:156n6]107j2{94L0?133p4}100l4@92j8/153B7}99u2?142o1;136N7[101S1:84F3$125t0&amp;107Q9{97u9;170X7=106F4}109l0*(191i8+189R1)201f0[197U2!200J8.203w7:(</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>35b6!T3:o1)J6^T3]H3$n8{o8&lt;;87b6!89T3:143o1)83J6^76T3]120H3$86n8{78o8&lt;;166l0)166U3+;</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10M1~N2[U7}F5|K1;q0=H1+h4.y4=j3.y3.*65M1~65N2[79U7}62F5|55K1;113q0=62H1+69h4.92y4=61j3.105y3.*197E4-197g4;197R3_*</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ññ</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>76k1@J0`q1}Z0/Z9&amp;m2@g1/t7&gt;{132k1@130J0`146q1}127Z0/114Z9&amp;153m2@127g1/171t7&gt;{327F3&amp;327M3_{</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>11m1}L6|R0[w0*O2?)60m1}65L6|132R0[68w0*57O2?)257y9.)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ñ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>62d9$M5&lt;R2{V4(g5!&amp;116d9$110M5&lt;128R2{118V4(125g5!&amp;301B8?&amp;</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>60d7%O5/T8}L9*L8&gt;:115d7%111O5/162T8}108L9*106L8&gt;:314f0.:</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>46m1+J3)b8!J1,w5,-101m1+101J3)158b8!97J1,108w5,-185p3&gt;-</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>95B2*H2^P7.R1&amp;P6|?146B2*151H2^177P7.149R1&amp;156P6|?146R6=?</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregado el frame private key y el frame successfully
</commit_message>
<xml_diff>
--- a/Password.xlsx
+++ b/Password.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="F1" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H1" s="3" t="inlineStr">
         <is>
@@ -471,85 +471,170 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>camilo</t>
+          <t>ññ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>37V9#A1&gt;P0%j4-i3/i4#X3[c4)g6%F2|b9)g9+i2`X2$T7)E0(s5-U6(K3]Y6;,87V9#90A1&gt;139P0%92j4-73i3/158i4#93X3[163c4)159g6%86F2|101b9)123g9+91i2`79X2$154T7)88E0(74s5-108U6(89K3]162Y6;,124f7$122y8~134z1@130V6*133u3%136G4},</t>
+          <t>76k1@J0`q1}Z0/Z9&amp;m2@g1/t7&gt;{132k1@130J0`146q1}127Z0/114Z9&amp;153m2@127g1/171t7&gt;{327F3&amp;327M3_{</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>51m0&gt;z2:n6]j2{L0?p4}l4@j8/B7}u2?o1;N7[S1:F3$t0&amp;Q9{u9;X7=F4}l0*(108m0&gt;101z2:156n6]107j2{94L0?133p4}100l4@92j8/153B7}99u2?142o1;136N7[101S1:84F3$125t0&amp;107Q9{97u9;170X7=106F4}109l0*(191i8+189R1)201f0[197U2!200J8.203w7:(</t>
+          <t>11m1}L6|R0[w0*O2?)60m1}65L6|132R0[68w0*57O2?)257y9.)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>camilo</t>
+          <t>ñ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>35b6!T3:o1)J6^T3]H3$n8{o8&lt;;87b6!89T3:143o1)83J6^76T3]120H3$86n8{78o8&lt;;166l0)166U3+;</t>
+          <t>62d9$M5&lt;R2{V4(g5!&amp;116d9$110M5&lt;128R2{118V4(125g5!&amp;301B8?&amp;</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10M1~N2[U7}F5|K1;q0=H1+h4.y4=j3.y3.*65M1~65N2[79U7}62F5|55K1;113q0=62H1+69h4.92y4=61j3.105y3.*197E4-197g4;197R3_*</t>
+          <t>60d7%O5/T8}L9*L8&gt;:115d7%111O5/162T8}108L9*106L8&gt;:314f0.:</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ññ</t>
+          <t>l</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>76k1@J0`q1}Z0/Z9&amp;m2@g1/t7&gt;{132k1@130J0`146q1}127Z0/114Z9&amp;153m2@127g1/171t7&gt;{327F3&amp;327M3_{</t>
+          <t>46m1+J3)b8!J1,w5,-101m1+101J3)158b8!97J1,108w5,-185p3&gt;-</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11m1}L6|R0[w0*O2?)60m1}65L6|132R0[68w0*57O2?)257y9.)</t>
+          <t>95B2*H2^P7.R1&amp;P6|?146B2*151H2^177P7.149R1&amp;156P6|?146R6=?</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ñ</t>
+          <t>camilo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>62d9$M5&lt;R2{V4(g5!&amp;116d9$110M5&lt;128R2{118V4(125g5!&amp;301B8?&amp;</t>
+          <t>66S8_l5@F8/X0-h1#m4$v7|A5=M0{W4|V8(W0?j5&gt;q5+A4-L7~K8&amp;t7;a4)Q8~[117S8_121l5@149F8/119X0-192h1#132m4$118v7|160A5=146M0{120W4|112V8(177W0?117j5&gt;128q5+167A4-118L7~110K8&amp;174t7;116a4)190Q8~[136S5~134B4^146P6.142o3&gt;145e4,148l2|[</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>60d7%O5/T8}L9*L8&gt;:115d7%111O5/162T8}108L9*106L8&gt;:314f0.:</t>
+          <t>87q7*D4&amp;K1!e6$m0?M3&amp;c3_f5!l4&amp;X4&gt;x9*A6_y9:w8;z0]q0|M4.h1$o1:p9&gt;@138q7*144D4&amp;201K1!141e6$132m0?152M3&amp;144c3_213f5!177l4&amp;136X4&gt;120x9*208A6_140y9:150w8;166z0]138q0|178M4.163h1$142o1:150p9&gt;@138r6-136A9~148Z1!144y5?147O3[150L7?@</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>camilo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>46m1+J3)b8!J1,w5,-101m1+101J3)158b8!97J1,108w5,-185p3&gt;-</t>
+          <t>63H0&amp;F6{W4@i5]G6:m3_m8!J2[A1&amp;N0_W4]l6+I8_n2#A0|s4)o1%S2?J1-K2#`118H0&amp;118F6{167W4@117i5]186G6:130m3_116m8!96J2[128A1&amp;118N0_157W4]148l6+113I8_158n2#141A0|111s4)109o1%167S2?118J1-125K2#`176h6{174C5!186A7^182U2_185N0.188h7&gt;`</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>95B2*H2^P7.R1&amp;P6|?146B2*151H2^177P7.149R1&amp;156P6|?146R6=?</t>
+          <t>91b5:Z0;o5?O7|n9?l7`l9}T8)Y6|T3]P6&gt;Q6#Q6~e0(B3%W2,E7|A5}X3}m1;&lt;146b5:145Z0;164o5?147O7|216n9?158l7`147l9}153T8)178Y6|143T3]131P6&gt;181Q6#140Q6~150e0(165B3%145W2,215E7|164A5}141X3}128m1;&lt;175I8}173C8&gt;185W4(181Z1;184J6|187I2%&lt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>34D6&amp;Z2_F0?d2{V1?I2#Y8|b9?v6#A6#a2]Q2|c7@s3(h7-w7?b5+r4!N0[F0}/91D6&amp;84Z2_110F0?86d2{74V1?99I2#91Y8|128b9?134v6#86A6#127a2]141Q2|85c7@71s3(144h7-88w7?70b5+133r4!83N0[157F0}/191L4(189A9^201d4]197k3%200n6$203c1{/</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>30e5`d8_s6|e1[v7^o5;b3`E9.F0~G8&lt;k1!m8~w3*d4-y8*R0=u1(D3,F8]M2:)83e5`83d8_96s6|79e1[121v7^131o5;84b3`70E9.107F0~86G8&lt;125k1!116m8~79w3*156d4-141y8*78R0=88u1(102D3,78F8]91M2:)154B1[152e6(164M8_160V1~163o0:166H0=)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>49i0:g3(K0:m0)H5!=98i0:102g3(155K0:106m0)82H5!=112j9!=</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>24W0@A8+m7:X9#A6~/80W0@74A8+144m7:75X9#67A6~/179x3+/</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13d0&amp;L9*A9,g4!S3_w1=D0$q4&amp;&lt;62d0&amp;66L9*113A9,67g4!74S3_102w1=62D0$76q4&amp;&lt;114d6=114Y1?&lt;</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>27D9[D2)P0}y7*M4.`84D9[82D2)126P0}76y7*89M4.`196c1&gt;`</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>37p8(N1&gt;z4.b7+c3~i5`z1+s8@^86p8(94N1&gt;102z4.93b7+98c3~139i5`94z1+97s8@^134A8=134f9&lt;^</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12a1.Q5[m4`c9,Q3`J9(Q0)A3~|65a1.61Q5[123m4`60c9,107Q3`125J9(66Q0)106A3~|148o0_148q6^|</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>26A8~M3{V1&gt;W9%f4=r9`w8+O0]r1_c8|L7~h2%z2~M4?b6+m1+H5-w3^f6@R4()80A8~76M3{108V1&gt;76W9%63f4=113r9`77w8+84O0]133r1_82c8|87L7~140h2%74z2~73M4?138b6+78m1+66H5-111w3^83f6@117R4()161R2%159W3:171k8=167r0/170p4(173U9[)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>46K2#R7*P2-Z5^v4$M2.O6|V3?r4~H1{A2-h4.y8&amp;y3~p5+I7`J0&lt;J5^l3&amp;Z7@!99K2#95R7*165P2-102Z5^140v4$125M2.102O6|86V3?146r4~103H1{172A2-154h4.97y8&amp;91y3~112p5+99I7`142J0&lt;144J5^103l3&amp;171Z7@!150w8^148O8(160d9~156l3-159B5`162b9}!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalizacion interfaz private key y se hicieron mejoras en el codigo
</commit_message>
<xml_diff>
--- a/Password.xlsx
+++ b/Password.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,6 +30,14 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -53,9 +61,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -426,16 +435,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="18.42578125" customWidth="1" style="4" min="2" max="2"/>
-    <col width="16.42578125" customWidth="1" style="4" min="3" max="3"/>
+    <col width="18.42578125" customWidth="1" style="5" min="2" max="2"/>
+    <col width="16.42578125" customWidth="1" style="5" min="3" max="3"/>
+    <col width="12.5703125" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -460,183 +470,45 @@
         </is>
       </c>
       <c r="F1" t="n">
-        <v>17</v>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>El valor de counter indica la posicion libre en la que se pondra el siguiente dominio, email etc</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ññ</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>76k1@J0`q1}Z0/Z9&amp;m2@g1/t7&gt;{132k1@130J0`146q1}127Z0/114Z9&amp;153m2@127g1/171t7&gt;{327F3&amp;327M3_{</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>11m1}L6|R0[w0*O2?)60m1}65L6|132R0[68w0*57O2?)257y9.)</t>
+    <row r="2">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>PrivateKey:</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>57a0!c0&gt;u2.r4(c9-r4#l2^x0~O7*P3}K9-C9#m8,w4+z0*Y7+A4-P8*I7{v1^=114a0!107c0&gt;138u2.111r4(119c9-179r4#110l2^100x0~177O7*107P3}150K9-128C9#113m8,183w4+162z0*105Y7+181A4-128P8*110I7{102v1^=191Q6&gt;189z5+201x2]197G8~200i0|203G5-=</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ñ</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>62d9$M5&lt;R2{V4(g5!&amp;116d9$110M5&lt;128R2{118V4(125g5!&amp;301B8?&amp;</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>60d7%O5/T8}L9*L8&gt;:115d7%111O5/162T8}108L9*106L8&gt;:314f0.:</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>46m1+J3)b8!J1,w5,-101m1+101J3)158b8!97J1,108w5,-185p3&gt;-</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>95B2*H2^P7.R1&amp;P6|?146B2*151H2^177P7.149R1&amp;156P6|?146R6=?</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>camilo</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>66S8_l5@F8/X0-h1#m4$v7|A5=M0{W4|V8(W0?j5&gt;q5+A4-L7~K8&amp;t7;a4)Q8~[117S8_121l5@149F8/119X0-192h1#132m4$118v7|160A5=146M0{120W4|112V8(177W0?117j5&gt;128q5+167A4-118L7~110K8&amp;174t7;116a4)190Q8~[136S5~134B4^146P6.142o3&gt;145e4,148l2|[</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>87q7*D4&amp;K1!e6$m0?M3&amp;c3_f5!l4&amp;X4&gt;x9*A6_y9:w8;z0]q0|M4.h1$o1:p9&gt;@138q7*144D4&amp;201K1!141e6$132m0?152M3&amp;144c3_213f5!177l4&amp;136X4&gt;120x9*208A6_140y9:150w8;166z0]138q0|178M4.163h1$142o1:150p9&gt;@138r6-136A9~148Z1!144y5?147O3[150L7?@</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>camilo</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>63H0&amp;F6{W4@i5]G6:m3_m8!J2[A1&amp;N0_W4]l6+I8_n2#A0|s4)o1%S2?J1-K2#`118H0&amp;118F6{167W4@117i5]186G6:130m3_116m8!96J2[128A1&amp;118N0_157W4]148l6+113I8_158n2#141A0|111s4)109o1%167S2?118J1-125K2#`176h6{174C5!186A7^182U2_185N0.188h7&gt;`</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>91b5:Z0;o5?O7|n9?l7`l9}T8)Y6|T3]P6&gt;Q6#Q6~e0(B3%W2,E7|A5}X3}m1;&lt;146b5:145Z0;164o5?147O7|216n9?158l7`147l9}153T8)178Y6|143T3]131P6&gt;181Q6#140Q6~150e0(165B3%145W2,215E7|164A5}141X3}128m1;&lt;175I8}173C8&gt;185W4(181Z1;184J6|187I2%&lt;</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>camilo</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>34D6&amp;Z2_F0?d2{V1?I2#Y8|b9?v6#A6#a2]Q2|c7@s3(h7-w7?b5+r4!N0[F0}/91D6&amp;84Z2_110F0?86d2{74V1?99I2#91Y8|128b9?134v6#86A6#127a2]141Q2|85c7@71s3(144h7-88w7?70b5+133r4!83N0[157F0}/191L4(189A9^201d4]197k3%200n6$203c1{/</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>30e5`d8_s6|e1[v7^o5;b3`E9.F0~G8&lt;k1!m8~w3*d4-y8*R0=u1(D3,F8]M2:)83e5`83d8_96s6|79e1[121v7^131o5;84b3`70E9.107F0~86G8&lt;125k1!116m8~79w3*156d4-141y8*78R0=88u1(102D3,78F8]91M2:)154B1[152e6(164M8_160V1~163o0:166H0=)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>49i0:g3(K0:m0)H5!=98i0:102g3(155K0:106m0)82H5!=112j9!=</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>24W0@A8+m7:X9#A6~/80W0@74A8+144m7:75X9#67A6~/179x3+/</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>72b4]t9.F8}O6,N9]Y8{K0|Y3#x1]k3|s8)T2!P6:N1&amp;O8(c4!C5|n3,v1`i2]^128b4]128t9.147F8}120O6,110N9]192Y8{128K0|197Y3#137x1]127k3|109s8)158T2!125P6:133N1&amp;184O8(129c4!163C5|160n3,126v1`196i2]^187K0&amp;185x8}197A7%193V5=196p9[199X6|^</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>20w5|c6/Q2]D0_G9)x6}H2!Z4#K2_e8&lt;I6-h7+P7.i4*g8}k9.u3,B4[C5)D0]@71w5|70c6/107Q2]70D0_66G9)123x6}69H2!61Z4#129K2_71e8&lt;78I6-124h7+69P7.78i4*90g8}69k9.81u3,100B4[75C5)61D0]@131W2.129g1)141m3:137h1:140F1=143P7)@</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ccc</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>13d0&amp;L9*A9,g4!S3_w1=D0$q4&amp;&lt;62d0&amp;66L9*113A9,67g4!74S3_102w1=62D0$76q4&amp;&lt;114d6=114Y1?&lt;</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>27D9[D2)P0}y7*M4.`84D9[82D2)126P0}76y7*89M4.`196c1&gt;`</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>dd</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>37p8(N1&gt;z4.b7+c3~i5`z1+s8@^86p8(94N1&gt;102z4.93b7+98c3~139i5`94z1+97s8@^134A8=134f9&lt;^</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>12a1.Q5[m4`c9,Q3`J9(Q0)A3~|65a1.61Q5[123m4`60c9,107Q3`125J9(66Q0)106A3~|148o0_148q6^|</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>camilo</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>26A8~M3{V1&gt;W9%f4=r9`w8+O0]r1_c8|L7~h2%z2~M4?b6+m1+H5-w3^f6@R4()80A8~76M3{108V1&gt;76W9%63f4=113r9`77w8+84O0]133r1_82c8|87L7~140h2%74z2~73M4?138b6+78m1+66H5-111w3^83f6@117R4()161R2%159W3:171k8=167r0/170p4(173U9[)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>46K2#R7*P2-Z5^v4$M2.O6|V3?r4~H1{A2-h4.y8&amp;y3~p5+I7`J0&lt;J5^l3&amp;Z7@!99K2#95R7*165P2-102Z5^140v4$125M2.102O6|86V3?146r4~103H1{172A2-154h4.97y8&amp;91y3~112p5+99I7`142J0&lt;144J5^103l3&amp;171Z7@!150w8^148O8(160d9~156l3-159B5`162b9}!</t>
-        </is>
-      </c>
+      <c r="F11" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Quitando pruebas del archivo password
</commit_message>
<xml_diff>
--- a/Password.xlsx
+++ b/Password.xlsx
@@ -1,49 +1,73 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GItHub\Save-passwords\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Email/Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Counter:</t>
+  </si>
+  <si>
+    <t>PrivateKey:</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -62,87 +86,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -430,85 +395,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="18.42578125" customWidth="1" style="5" min="2" max="2"/>
-    <col width="16.42578125" customWidth="1" style="5" min="3" max="3"/>
-    <col width="12.5703125" customWidth="1" style="5" min="5" max="5"/>
+    <col min="2" max="2" width="18.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Domain</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Email/Username</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Counter:</t>
-        </is>
-      </c>
-      <c r="F1" t="n">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>El valor de counter indica la posicion libre en la que se pondra el siguiente dominio, email etc</t>
-        </is>
-      </c>
     </row>
-    <row r="2">
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>PrivateKey:</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>57a0!c0&gt;u2.r4(c9-r4#l2^x0~O7*P3}K9-C9#m8,w4+z0*Y7+A4-P8*I7{v1^=114a0!107c0&gt;138u2.111r4(119c9-179r4#110l2^100x0~177O7*107P3}150K9-128C9#113m8,183w4+162z0*105Y7+181A4-128P8*110I7{102v1^=191Q6&gt;189z5+201x2]197G8~200i0|203G5-=</t>
-        </is>
-      </c>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3"/>
+      <c r="C3"/>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>camilo</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>72b4]t9.F8}O6,N9]Y8{K0|Y3#x1]k3|s8)T2!P6:N1&amp;O8(c4!C5|n3,v1`i2]^128b4]128t9.147F8}120O6,110N9]192Y8{128K0|197Y3#137x1]127k3|109s8)158T2!125P6:133N1&amp;184O8(129c4!163C5|160n3,126v1`196i2]^187K0&amp;185x8}197A7%193V5=196p9[199X6|^</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>20w5|c6/Q2]D0_G9)x6}H2!Z4#K2_e8&lt;I6-h7+P7.i4*g8}k9.u3,B4[C5)D0]@71w5|70c6/107Q2]70D0_66G9)123x6}69H2!61Z4#129K2_71e8&lt;78I6-124h7+69P7.78i4*90g8}69k9.81u3,100B4[75C5)61D0]@131W2.129g1)141m3:137h1:140F1=143P7)@</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="F11" s="2" t="n"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fixed delete password bug
</commit_message>
<xml_diff>
--- a/Password.xlsx
+++ b/Password.xlsx
@@ -1,73 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GItHub\Save-passwords\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>Email/Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Counter:</t>
-  </si>
-  <si>
-    <t>PrivateKey:</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -86,28 +62,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -395,59 +430,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col width="18.42578125" customWidth="1" style="5" min="2" max="2"/>
+    <col width="16.42578125" customWidth="1" style="5" min="3" max="3"/>
+    <col width="12.5703125" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Domain</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email/Username</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Counter:</t>
+        </is>
+      </c>
+      <c r="F1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="n"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
-        <v>4</v>
+    <row r="2">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>PrivateKey:</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>36D7/f4{F5:K1/H8&amp;|85D7/88f4{107F5:85K1/100H8&amp;|113G1@|</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3"/>
-      <c r="C3"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F11" s="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10">
+      <c r="F10" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>